<commit_message>
correzioni varie generazione report collaboratori
</commit_message>
<xml_diff>
--- a/static/report_collaboratori_compilato.xlsx
+++ b/static/report_collaboratori_compilato.xlsx
@@ -468,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,26 +519,608 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>11/09/2023</t>
+          <t>01/08/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0006</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Supporti</t>
+          <t>000B</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Gestione Società</t>
         </is>
       </c>
       <c r="E2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>03/08/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>000B</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Gestione Società</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>04/08/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>000B</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Gestione Società</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>07/08/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Stress Analysis</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>07/08/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>000B</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Gestione Società</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>08/08/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Stress Analysis</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>16/08/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Stress Analysis</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>16/08/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>000B</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Gestione Società</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>17/08/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Stress Analysis</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>21/08/2023</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Stress Analysis</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
         <v>4</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>21/08/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>000B</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Gestione Società</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>22/08/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Stress Analysis</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>23/08/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Stress Analysis</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>24/08/2023</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Stress Analysis</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>24/08/2023</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>25/08/2023</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>25/08/2023</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>000B</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Gestione Società</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>04/09/2023</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>000B</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Gestione Società</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>05/09/2023</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>05/09/2023</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>000B</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Gestione Società</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>07/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>07/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>000B</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Gestione Società</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -618,7 +1200,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,6 +1248,126 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01/08/2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>01/08/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>02/08/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>02/08/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -679,7 +1381,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -727,6 +1429,576 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01/08/2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>02/08/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>03/08/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>07/08/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>9</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>08/08/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>9</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>09/08/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>10/08/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>11/08/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>14/08/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>16/08/2023</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>8</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>17/08/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>8</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>8</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>21/08/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>22/08/2023</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>23/08/2023</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>24/08/2023</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>25/08/2023</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>28/08/2023</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>10</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>29/08/2023</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Dromont - 22002</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -740,7 +2012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -788,6 +2060,816 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01/08/2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0005</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Team Project - MINO</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>02/08/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0005</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Team Project - MINO</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>03/08/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0005</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Team Project - MINO</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>04/08/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0005</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Team Project - MINO</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>07/08/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>08/08/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>09/08/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>10/08/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>16/08/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>17/08/2023</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>8</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>8</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>21/08/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>8</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>22/08/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>7</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>23/08/2023</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>9</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>24/08/2023</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>8</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>25/08/2023</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>28/08/2023</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>29/08/2023</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>30/08/2023</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>8</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>31/08/2023</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>8</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>8</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>04/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0006</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Skid S051 nuova linea</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>8</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>05/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0006</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Skid S051 nuova linea</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>6</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>06/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>06/09/2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0005</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Team Project - MINO</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>6</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>07/09/2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0005</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Team Project - MINO</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>8</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>08/09/2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>0005</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Team Project - MINO</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>8</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -801,7 +2883,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,6 +2931,726 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01/08/2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>02/08/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>03/08/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>04/08/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>07/08/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>08/08/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>09/08/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>10/08/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>11/08/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>17/08/2023</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>8</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>18/08/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>21/08/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>8</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>22/08/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>23/08/2023</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>8</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>24/08/2023</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>6</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>28/08/2023</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>04/09/2023</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>05/09/2023</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>8</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>06/09/2023</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>8</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>07/09/2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>07/09/2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>4</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>08/09/2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>8</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>11/09/2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0004</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>GRS</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>8</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -862,7 +3664,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -910,6 +3712,516 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>07/08/2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>08/08/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>09/08/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>10/08/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>11/08/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>21/08/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>7</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>22/08/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>23/08/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>24/08/2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>25/08/2023</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>29/08/2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>8</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01/09/2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>04/09/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>05/09/2023</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>8</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>06/09/2023</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>8</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>07/09/2023</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08/09/2023</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>3222</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Piping</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>6</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>